<commit_message>
making it a loop and saving variables in each increment
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -1,53 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Order #</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Pizza Type</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <color theme="1"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
@@ -57,25 +38,87 @@
     <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -273,44 +316,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="27.88"/>
-    <col customWidth="1" min="3" max="3" width="39.63"/>
-    <col customWidth="1" min="4" max="4" width="31.88"/>
-    <col customWidth="1" min="5" max="5" width="20.63"/>
+    <col width="27.88" customWidth="1" style="2" min="2" max="2"/>
+    <col width="39.63" customWidth="1" style="2" min="3" max="3"/>
+    <col width="31.88" customWidth="1" style="2" min="4" max="4"/>
+    <col width="20.63" customWidth="1" style="2" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Order #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Pizza Type</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>2.0</v>
+      <c r="A2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>djdj</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>cnskm@ndien</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>113.685</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added tyes of pizza to transaction
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,7 +321,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -331,8 +331,11 @@
   <cols>
     <col width="27.88" customWidth="1" style="2" min="2" max="2"/>
     <col width="39.63" customWidth="1" style="2" min="3" max="3"/>
-    <col width="31.88" customWidth="1" style="2" min="4" max="4"/>
-    <col width="20.63" customWidth="1" style="2" min="5" max="5"/>
+    <col width="21.63" customWidth="1" style="2" min="4" max="4"/>
+    <col width="20.13" customWidth="1" style="2" min="5" max="5"/>
+    <col width="23.25" customWidth="1" style="2" min="6" max="6"/>
+    <col width="31.88" customWidth="1" style="2" min="7" max="7"/>
+    <col width="20.63" customWidth="1" style="2" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -353,10 +356,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Pizza Type</t>
+          <t>Cheese Pizzas</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Pepperoni Pizzas</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Hawaiian Pizzas</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Meat Lovers Pizzas</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -376,8 +394,20 @@
           <t>s</t>
         </is>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E2" s="0" t="n">
-        <v>52.5525</v>
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" t="n">
+        <v>149.0775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get values from excel
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,28 +386,28 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>balls</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>bals@yahoo.com</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H2" t="n">
-        <v>149.0775</v>
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>34.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a way to get values from execl for pizzas
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,28 +386,28 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>balls</t>
+          <t>d</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>bals@yahoo.com</t>
+          <t>d</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>34.32</v>
+        <v>48.2625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on checkout screen
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,7 +321,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -386,19 +386,19 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>w</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>w</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
@@ -407,7 +407,12 @@
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>48.2625</v>
+        <v>18.2325</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checkout screen shows pizzas now
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,28 +386,28 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>w</t>
+          <t>d</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>w</t>
+          <t>d</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="H2" s="0" t="n">
-        <v>18.2325</v>
+        <v>269.1975</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
total is rounded now
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,28 +386,28 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>s</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="G2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>269.1975</v>
+        <v>34.32</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
need to make main window run everything through input
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,28 +386,28 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>d</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>d</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>34.32</v>
+        <v>54.7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
tried to make it executable
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,12 +386,12 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>diego</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>fnjrdrn@gmail</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
@@ -404,10 +404,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>54.7</v>
+        <v>95.45</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
retrieved pizzas for first order from excel for chef
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,12 +386,12 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>d</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>d</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
@@ -401,13 +401,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>34.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
made customer transaction loop successfully, only need to make the cus id work correclt and get the right values from excel back
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,19 +386,19 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>and</t>
+          <t>s</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>ans@nfinf</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
@@ -407,7 +407,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>97.59999999999999</v>
+        <v>61.13</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
find way to do if statement after class completion to call chekcout class
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -327,7 +327,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="27.88" customWidth="1" style="2" min="2" max="2"/>
     <col width="39.63" customWidth="1" style="2" min="3" max="3"/>
@@ -386,28 +386,28 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>die</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>nes</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>61.13</v>
+        <v>109.4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
customer transactions basic functions have been finished, need to make loop put new order on a new line in excel and it will be fully functional
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -382,37 +382,62 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>die</t>
+          <t>ser</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>nes</t>
+          <t>e</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>109.4</v>
+        <v>48.26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>aaaa</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>468.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made a transaction reset method for manager
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,13 +321,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="27.88" customWidth="1" style="2" min="2" max="2"/>
     <col width="39.63" customWidth="1" style="2" min="3" max="3"/>
@@ -384,246 +384,9 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>diego</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>rhr</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>804.38</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>32.17</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>48.26</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>64.34999999999999</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>i</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>j</t>
-        </is>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>80.44</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>96.52</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>u</t>
-        </is>
-      </c>
-      <c r="C8" s="0" t="inlineStr">
-        <is>
-          <t>u</t>
-        </is>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>128.7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="C9" s="0" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>144.79</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="n">
-        <v>10</v>
-      </c>
+      <c r="A4" s="0" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
made main sign in for cusotmer employee and manager
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,7 +321,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,14 +384,22 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="B2" s="0" t="n"/>
+      <c r="C2" s="0" t="n"/>
+      <c r="D2" s="0" t="n"/>
+      <c r="E2" s="0" t="n"/>
+      <c r="F2" s="0" t="n"/>
+      <c r="G2" s="0" t="n"/>
+      <c r="H2" s="0" t="n"/>
     </row>
-    <row r="3"/>
+    <row r="3">
+      <c r="A3" s="0" t="n"/>
+    </row>
     <row r="4">
       <c r="A4" s="0" t="n"/>
     </row>
     <row r="5"/>
     <row r="6"/>
-    <row r="7"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
employee sign in working
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,7 +321,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -394,12 +394,18 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="n"/>
+      <c r="B3" s="0" t="n"/>
+      <c r="C3" s="0" t="n"/>
+      <c r="D3" s="0" t="n"/>
+      <c r="E3" s="0" t="n"/>
+      <c r="F3" s="0" t="n"/>
+      <c r="G3" s="0" t="n"/>
+      <c r="H3" s="0" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="0" t="n"/>
     </row>
     <row r="5"/>
-    <row r="6"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
revenue needs to be implemented for manger hom epage
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,7 +321,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,16 +384,36 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n"/>
-      <c r="C2" s="0" t="n"/>
-      <c r="D2" s="0" t="n"/>
-      <c r="E2" s="0" t="n"/>
-      <c r="F2" s="0" t="n"/>
-      <c r="G2" s="0" t="n"/>
-      <c r="H2" s="0" t="n"/>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>er</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>36.47</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n"/>
+      <c r="A3" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="B3" s="0" t="n"/>
       <c r="C3" s="0" t="n"/>
       <c r="D3" s="0" t="n"/>
@@ -405,7 +425,6 @@
     <row r="4">
       <c r="A4" s="0" t="n"/>
     </row>
-    <row r="5"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
get revenue woks for manager class
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,7 +386,7 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>er</t>
+          <t>e</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
@@ -395,10 +395,10 @@
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
@@ -407,23 +407,43 @@
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>36.47</v>
+        <v>48.26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n"/>
-      <c r="C3" s="0" t="n"/>
-      <c r="D3" s="0" t="n"/>
-      <c r="E3" s="0" t="n"/>
-      <c r="F3" s="0" t="n"/>
-      <c r="G3" s="0" t="n"/>
-      <c r="H3" s="0" t="n"/>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>cf</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>583.4400000000001</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n"/>
+      <c r="A4" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
revenue shows on manager home page, next thing is to show total in checkoutscreen
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,7 +321,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,67 +384,38 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>48.26</v>
-      </c>
+      <c r="B2" s="0" t="n"/>
+      <c r="C2" s="0" t="n"/>
+      <c r="D2" s="0" t="n"/>
+      <c r="E2" s="0" t="n"/>
+      <c r="F2" s="0" t="n"/>
+      <c r="G2" s="0" t="n"/>
+      <c r="H2" s="0" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>cf</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>583.4400000000001</v>
-      </c>
+      <c r="A3" s="0" t="n"/>
+      <c r="B3" s="0" t="n"/>
+      <c r="C3" s="0" t="n"/>
+      <c r="D3" s="0" t="n"/>
+      <c r="E3" s="0" t="n"/>
+      <c r="F3" s="0" t="n"/>
+      <c r="G3" s="0" t="n"/>
+      <c r="H3" s="0" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n">
-        <v>4</v>
-      </c>
+      <c r="A4" s="0" t="n"/>
+      <c r="B4" s="0" t="n"/>
+      <c r="C4" s="0" t="n"/>
+      <c r="D4" s="0" t="n"/>
+      <c r="E4" s="0" t="n"/>
+      <c r="F4" s="0" t="n"/>
+      <c r="G4" s="0" t="n"/>
+      <c r="H4" s="0" t="n"/>
     </row>
+    <row r="5">
+      <c r="A5" s="0" t="n"/>
+    </row>
+    <row r="6"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
total get shown at chekcout and inventory is updated after checkout
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,7 +321,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,16 +384,36 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n"/>
-      <c r="C2" s="0" t="n"/>
-      <c r="D2" s="0" t="n"/>
-      <c r="E2" s="0" t="n"/>
-      <c r="F2" s="0" t="n"/>
-      <c r="G2" s="0" t="n"/>
-      <c r="H2" s="0" t="n"/>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>3217.5</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n"/>
+      <c r="A3" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="B3" s="0" t="n"/>
       <c r="C3" s="0" t="n"/>
       <c r="D3" s="0" t="n"/>
@@ -415,7 +435,6 @@
     <row r="5">
       <c r="A5" s="0" t="n"/>
     </row>
-    <row r="6"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added manager closing kiosk functionality
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,7 +321,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -386,16 +386,16 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>u</t>
+          <t>e</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>p</t>
+          <t>e</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
@@ -407,33 +407,83 @@
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>3217.5</v>
+        <v>16.09</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n"/>
-      <c r="C3" s="0" t="n"/>
-      <c r="D3" s="0" t="n"/>
-      <c r="E3" s="0" t="n"/>
-      <c r="F3" s="0" t="n"/>
-      <c r="G3" s="0" t="n"/>
-      <c r="H3" s="0" t="n"/>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>er</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>32.17</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n"/>
-      <c r="B4" s="0" t="n"/>
-      <c r="C4" s="0" t="n"/>
-      <c r="D4" s="0" t="n"/>
-      <c r="E4" s="0" t="n"/>
-      <c r="F4" s="0" t="n"/>
-      <c r="G4" s="0" t="n"/>
-      <c r="H4" s="0" t="n"/>
+      <c r="A4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>edd</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2222</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>35746.42</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="n"/>
+      <c r="A5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n"/>
+      <c r="C5" s="0" t="n"/>
+      <c r="D5" s="0" t="n"/>
+      <c r="E5" s="0" t="n"/>
+      <c r="F5" s="0" t="n"/>
+      <c r="G5" s="0" t="n"/>
+      <c r="H5" s="0" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
making program look better
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -386,49 +386,47 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>d</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>d</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>36.47</v>
+        <v>51.48</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>3</v>
-      </c>
+      <c r="A3" s="0" t="n"/>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>er</t>
+          <t>r</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>r</t>
         </is>
       </c>
       <c r="D3" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
@@ -437,43 +435,23 @@
         <v>0</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>32.17</v>
+        <v>91.16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>edd</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>ddd</t>
-        </is>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>2222</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>35746.42</v>
-      </c>
+      <c r="B4" s="0" t="n"/>
+      <c r="C4" s="0" t="n"/>
+      <c r="D4" s="0" t="n"/>
+      <c r="E4" s="0" t="n"/>
+      <c r="F4" s="0" t="n"/>
+      <c r="G4" s="0" t="n"/>
+      <c r="H4" s="0" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="n">
-        <v>5</v>
-      </c>
+      <c r="A5" s="0" t="n"/>
       <c r="B5" s="0" t="n"/>
       <c r="C5" s="0" t="n"/>
       <c r="D5" s="0" t="n"/>

</xml_diff>

<commit_message>
more fron tend design
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,13 +321,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="27.88" customWidth="1" style="2" min="2" max="2"/>
     <col width="39.63" customWidth="1" style="2" min="3" max="3"/>
@@ -384,64 +384,26 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>51.48</v>
-      </c>
+      <c r="B2" s="0" t="n"/>
+      <c r="C2" s="0" t="n"/>
+      <c r="D2" s="0" t="n"/>
+      <c r="E2" s="0" t="n"/>
+      <c r="F2" s="0" t="n"/>
+      <c r="G2" s="0" t="n"/>
+      <c r="H2" s="0" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n"/>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>91.16</v>
-      </c>
+      <c r="B3" s="0" t="n"/>
+      <c r="C3" s="0" t="n"/>
+      <c r="D3" s="0" t="n"/>
+      <c r="E3" s="0" t="n"/>
+      <c r="F3" s="0" t="n"/>
+      <c r="G3" s="0" t="n"/>
+      <c r="H3" s="0" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n">
-        <v>4</v>
-      </c>
+      <c r="A4" s="0" t="n"/>
       <c r="B4" s="0" t="n"/>
       <c r="C4" s="0" t="n"/>
       <c r="D4" s="0" t="n"/>
@@ -463,6 +425,9 @@
     <row r="6">
       <c r="A6" s="0" t="n"/>
     </row>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
better design to the interface manager
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -321,7 +321,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,13 +384,31 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n"/>
-      <c r="C2" s="0" t="n"/>
-      <c r="D2" s="0" t="n"/>
-      <c r="E2" s="0" t="n"/>
-      <c r="F2" s="0" t="n"/>
-      <c r="G2" s="0" t="n"/>
-      <c r="H2" s="0" t="n"/>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>54.7</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n"/>
@@ -425,8 +443,6 @@
     <row r="6">
       <c r="A6" s="0" t="n"/>
     </row>
-    <row r="7"/>
-    <row r="8"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
interface fixed on manager
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -384,31 +384,13 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>54.7</v>
-      </c>
+      <c r="B2" s="0" t="n"/>
+      <c r="C2" s="0" t="n"/>
+      <c r="D2" s="0" t="n"/>
+      <c r="E2" s="0" t="n"/>
+      <c r="F2" s="0" t="n"/>
+      <c r="G2" s="0" t="n"/>
+      <c r="H2" s="0" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n"/>

</xml_diff>

<commit_message>
no total can equal 0
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -391,11 +391,11 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>s</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
@@ -407,15 +407,23 @@
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>64.34999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n"/>
-      <c r="C3" s="0" t="n"/>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
       <c r="D3" s="0" t="n"/>
       <c r="E3" s="0" t="n"/>
       <c r="F3" s="0" t="n"/>

</xml_diff>

<commit_message>
documentation only needed for runner sing in and chef sign in now
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -384,96 +384,36 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>36.47</v>
-      </c>
+      <c r="B2" s="0" t="n"/>
+      <c r="C2" s="0" t="n"/>
+      <c r="D2" s="0" t="n"/>
+      <c r="E2" s="0" t="n"/>
+      <c r="F2" s="0" t="n"/>
+      <c r="G2" s="0" t="n"/>
+      <c r="H2" s="0" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>213.43</v>
-      </c>
+      <c r="A3" s="0" t="n"/>
+      <c r="B3" s="0" t="n"/>
+      <c r="C3" s="0" t="n"/>
+      <c r="D3" s="0" t="n"/>
+      <c r="E3" s="0" t="n"/>
+      <c r="F3" s="0" t="n"/>
+      <c r="G3" s="0" t="n"/>
+      <c r="H3" s="0" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>ert</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>tt</t>
-        </is>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>68.64</v>
-      </c>
+      <c r="A4" s="0" t="n"/>
+      <c r="B4" s="0" t="n"/>
+      <c r="C4" s="0" t="n"/>
+      <c r="D4" s="0" t="n"/>
+      <c r="E4" s="0" t="n"/>
+      <c r="F4" s="0" t="n"/>
+      <c r="G4" s="0" t="n"/>
+      <c r="H4" s="0" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="n">
-        <v>5</v>
-      </c>
+      <c r="A5" s="0" t="n"/>
       <c r="B5" s="0" t="n"/>
       <c r="C5" s="0" t="n"/>
       <c r="D5" s="0" t="n"/>

</xml_diff>

<commit_message>
changed backround menu, menu color, and subtitles
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -327,7 +327,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="27.88" customWidth="1" style="2" min="2" max="2"/>
     <col width="39.63" customWidth="1" style="2" min="3" max="3"/>
@@ -391,7 +391,7 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>zachcm19@GMAIL.CO</t>
+          <t>z</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">

</xml_diff>

<commit_message>
changinf main running file
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -327,7 +327,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="27.88" customWidth="1" style="2" min="2" max="2"/>
     <col width="39.63" customWidth="1" style="2" min="3" max="3"/>
@@ -386,44 +386,64 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>z</t>
+          <t>di</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>z</t>
+          <t>d</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>40.76</v>
+        <v>619.91</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n"/>
-      <c r="C3" s="0" t="n"/>
-      <c r="D3" s="0" t="n"/>
-      <c r="E3" s="0" t="n"/>
-      <c r="F3" s="0" t="n"/>
-      <c r="G3" s="0" t="n"/>
-      <c r="H3" s="0" t="n"/>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>rrt</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>51.48</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n"/>
+      <c r="A4" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B4" s="0" t="n"/>
       <c r="C4" s="0" t="n"/>
       <c r="D4" s="0" t="n"/>

</xml_diff>

<commit_message>
loop is better and exeption for order is fixed
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -384,66 +384,26 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>di</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>619.91</v>
-      </c>
+      <c r="B2" s="0" t="n"/>
+      <c r="C2" s="0" t="n"/>
+      <c r="D2" s="0" t="n"/>
+      <c r="E2" s="0" t="n"/>
+      <c r="F2" s="0" t="n"/>
+      <c r="G2" s="0" t="n"/>
+      <c r="H2" s="0" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>dd</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>rrt</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>51.48</v>
-      </c>
+      <c r="A3" s="0" t="n"/>
+      <c r="B3" s="0" t="n"/>
+      <c r="C3" s="0" t="n"/>
+      <c r="D3" s="0" t="n"/>
+      <c r="E3" s="0" t="n"/>
+      <c r="F3" s="0" t="n"/>
+      <c r="G3" s="0" t="n"/>
+      <c r="H3" s="0" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n">
-        <v>4</v>
-      </c>
+      <c r="A4" s="0" t="n"/>
       <c r="B4" s="0" t="n"/>
       <c r="C4" s="0" t="n"/>
       <c r="D4" s="0" t="n"/>

</xml_diff>

<commit_message>
class import in method
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -327,7 +327,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col width="27.88" customWidth="1" style="2" min="2" max="2"/>
     <col width="39.63" customWidth="1" style="2" min="3" max="3"/>
@@ -384,8 +384,16 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n"/>
-      <c r="C2" s="0" t="n"/>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>hh</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
       <c r="D2" s="0" t="n"/>
       <c r="E2" s="0" t="n"/>
       <c r="F2" s="0" t="n"/>

</xml_diff>

<commit_message>
testing logic for checkout screen
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -327,7 +327,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
   <cols>
     <col width="27.88" customWidth="1" style="2" min="2" max="2"/>
     <col width="39.63" customWidth="1" style="2" min="3" max="3"/>
@@ -386,32 +386,64 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>hh</t>
+          <t>e</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="n"/>
-      <c r="E2" s="0" t="n"/>
-      <c r="F2" s="0" t="n"/>
-      <c r="G2" s="0" t="n"/>
-      <c r="H2" s="0" t="n"/>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>48.26</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n"/>
-      <c r="B3" s="0" t="n"/>
-      <c r="C3" s="0" t="n"/>
-      <c r="D3" s="0" t="n"/>
-      <c r="E3" s="0" t="n"/>
-      <c r="F3" s="0" t="n"/>
-      <c r="G3" s="0" t="n"/>
-      <c r="H3" s="0" t="n"/>
+      <c r="A3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>16.09</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n"/>
+      <c r="A4" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B4" s="0" t="n"/>
       <c r="C4" s="0" t="n"/>
       <c r="D4" s="0" t="n"/>

</xml_diff>

<commit_message>
employee sign in and manager sign in loop correctly
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -391,7 +391,7 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>@icloud.com</t>
+          <t>@gmail.com</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
@@ -411,129 +411,47 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>dd</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>213.43</v>
-      </c>
+      <c r="A3" s="0" t="n"/>
+      <c r="B3" s="0" t="n"/>
+      <c r="C3" s="0" t="n"/>
+      <c r="D3" s="0" t="n"/>
+      <c r="E3" s="0" t="n"/>
+      <c r="F3" s="0" t="n"/>
+      <c r="G3" s="0" t="n"/>
+      <c r="H3" s="0" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>wer</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>@csun.edu</t>
-        </is>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>56.84</v>
-      </c>
+      <c r="A4" s="0" t="n"/>
+      <c r="B4" s="0" t="n"/>
+      <c r="C4" s="0" t="n"/>
+      <c r="D4" s="0" t="n"/>
+      <c r="E4" s="0" t="n"/>
+      <c r="F4" s="0" t="n"/>
+      <c r="G4" s="0" t="n"/>
+      <c r="H4" s="0" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>@gmail.com</t>
-        </is>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>56.84</v>
-      </c>
+      <c r="A5" s="0" t="n"/>
+      <c r="B5" s="0" t="n"/>
+      <c r="C5" s="0" t="n"/>
+      <c r="D5" s="0" t="n"/>
+      <c r="E5" s="0" t="n"/>
+      <c r="F5" s="0" t="n"/>
+      <c r="G5" s="0" t="n"/>
+      <c r="H5" s="0" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>@icloud.com</t>
-        </is>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>20.38</v>
-      </c>
+      <c r="A6" s="0" t="n"/>
+      <c r="B6" s="0" t="n"/>
+      <c r="C6" s="0" t="n"/>
+      <c r="D6" s="0" t="n"/>
+      <c r="E6" s="0" t="n"/>
+      <c r="F6" s="0" t="n"/>
+      <c r="G6" s="0" t="n"/>
+      <c r="H6" s="0" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="n">
-        <v>7</v>
-      </c>
+      <c r="A7" s="0" t="n"/>
       <c r="B7" s="0" t="n"/>
       <c r="C7" s="0" t="n"/>
       <c r="D7" s="0" t="n"/>

</xml_diff>

<commit_message>
refactoring for extra window done for both sprints, both start with files start1 and start2
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -384,186 +384,66 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>@gmail.com</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>68.64</v>
-      </c>
+      <c r="B2" s="0" t="n"/>
+      <c r="C2" s="0" t="n"/>
+      <c r="D2" s="0" t="n"/>
+      <c r="E2" s="0" t="n"/>
+      <c r="F2" s="0" t="n"/>
+      <c r="G2" s="0" t="n"/>
+      <c r="H2" s="0" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>48.26</v>
-      </c>
+      <c r="A3" s="0" t="n"/>
+      <c r="B3" s="0" t="n"/>
+      <c r="C3" s="0" t="n"/>
+      <c r="D3" s="0" t="n"/>
+      <c r="E3" s="0" t="n"/>
+      <c r="F3" s="0" t="n"/>
+      <c r="G3" s="0" t="n"/>
+      <c r="H3" s="0" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>@gmail.com</t>
-        </is>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>32.17</v>
-      </c>
+      <c r="A4" s="0" t="n"/>
+      <c r="B4" s="0" t="n"/>
+      <c r="C4" s="0" t="n"/>
+      <c r="D4" s="0" t="n"/>
+      <c r="E4" s="0" t="n"/>
+      <c r="F4" s="0" t="n"/>
+      <c r="G4" s="0" t="n"/>
+      <c r="H4" s="0" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>@gmail.com</t>
-        </is>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>48.26</v>
-      </c>
+      <c r="A5" s="0" t="n"/>
+      <c r="B5" s="0" t="n"/>
+      <c r="C5" s="0" t="n"/>
+      <c r="D5" s="0" t="n"/>
+      <c r="E5" s="0" t="n"/>
+      <c r="F5" s="0" t="n"/>
+      <c r="G5" s="0" t="n"/>
+      <c r="H5" s="0" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>@icloud.com</t>
-        </is>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>64.34999999999999</v>
-      </c>
+      <c r="A6" s="0" t="n"/>
+      <c r="B6" s="0" t="n"/>
+      <c r="C6" s="0" t="n"/>
+      <c r="D6" s="0" t="n"/>
+      <c r="E6" s="0" t="n"/>
+      <c r="F6" s="0" t="n"/>
+      <c r="G6" s="0" t="n"/>
+      <c r="H6" s="0" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>@gmail.com</t>
-        </is>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>71.86</v>
-      </c>
+      <c r="A7" s="0" t="n"/>
+      <c r="B7" s="0" t="n"/>
+      <c r="C7" s="0" t="n"/>
+      <c r="D7" s="0" t="n"/>
+      <c r="E7" s="0" t="n"/>
+      <c r="F7" s="0" t="n"/>
+      <c r="G7" s="0" t="n"/>
+      <c r="H7" s="0" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="n">
-        <v>8</v>
-      </c>
+      <c r="A8" s="0" t="n"/>
       <c r="B8" s="0" t="n"/>
       <c r="C8" s="0" t="n"/>
       <c r="D8" s="0" t="n"/>

</xml_diff>

<commit_message>
only need to have a rezise function and turn to executable
</commit_message>
<xml_diff>
--- a/customerTransactions.xlsx
+++ b/customerTransactions.xlsx
@@ -384,23 +384,61 @@
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n"/>
-      <c r="C2" s="0" t="n"/>
-      <c r="D2" s="0" t="n"/>
-      <c r="E2" s="0" t="n"/>
-      <c r="F2" s="0" t="n"/>
-      <c r="G2" s="0" t="n"/>
-      <c r="H2" s="0" t="n"/>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>71.86</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n"/>
-      <c r="B3" s="0" t="n"/>
-      <c r="C3" s="0" t="n"/>
-      <c r="D3" s="0" t="n"/>
-      <c r="E3" s="0" t="n"/>
-      <c r="F3" s="0" t="n"/>
-      <c r="G3" s="0" t="n"/>
-      <c r="H3" s="0" t="n"/>
+      <c r="A3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>16.09</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="n"/>

</xml_diff>